<commit_message>
Update kaspa_buys.xlsx after running on 2025-04-19
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -1,66 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding_stuff\crypto_buys\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A1C06E-278B-43B8-87DF-31BCF415BC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="750" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Coins</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>04/17/2025</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,45 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -401,170 +424,197 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Coins</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>45745</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>774.4</v>
       </c>
-      <c r="C2">
-        <v>6.3920000000000005E-2</v>
-      </c>
-      <c r="D2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="C2" t="n">
+        <v>0.06392</v>
+      </c>
+      <c r="D2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
         <v>45752</v>
       </c>
-      <c r="B3">
-        <v>771.67600000000004</v>
-      </c>
-      <c r="C3">
-        <v>6.4149999999999999E-2</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="B3" t="n">
+        <v>771.676</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.06415</v>
+      </c>
+      <c r="D3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
         <v>45752</v>
       </c>
-      <c r="B4">
-        <v>759.32</v>
-      </c>
-      <c r="C4">
-        <v>6.5199999999999994E-2</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="B4" t="n">
+        <v>759.3200000000001</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.06519999999999999</v>
+      </c>
+      <c r="D4" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
         <v>45752</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="n">
         <v>1542.222</v>
       </c>
-      <c r="C5">
-        <v>6.4199999999999993E-2</v>
-      </c>
-      <c r="D5">
+      <c r="C5" t="n">
+        <v>0.06419999999999999</v>
+      </c>
+      <c r="D5" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>45755</v>
       </c>
-      <c r="B6">
-        <v>803.60699999999997</v>
-      </c>
-      <c r="C6">
-        <v>6.1600000000000002E-2</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="B6" t="n">
+        <v>803.607</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0616</v>
+      </c>
+      <c r="D6" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
         <v>45757</v>
       </c>
-      <c r="B7">
-        <v>745.00199999999995</v>
-      </c>
-      <c r="C7">
-        <v>6.7110000000000003E-2</v>
-      </c>
-      <c r="D7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="B7" t="n">
+        <v>745.002</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.06711</v>
+      </c>
+      <c r="D7" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
         <v>45759</v>
       </c>
-      <c r="B8">
-        <v>664.76800000000003</v>
-      </c>
-      <c r="C8">
-        <v>7.5209999999999999E-2</v>
-      </c>
-      <c r="D8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="B8" t="n">
+        <v>664.768</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.07521</v>
+      </c>
+      <c r="D8" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
         <v>45762</v>
       </c>
-      <c r="B9">
-        <v>646.20399999999995</v>
-      </c>
-      <c r="C9">
-        <v>7.7369999999999994E-2</v>
-      </c>
-      <c r="D9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>647.21307999999954</v>
-      </c>
-      <c r="C10">
-        <v>7.7254310126118025E-2</v>
-      </c>
-      <c r="D10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="B9" t="n">
+        <v>646.204</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.07736999999999999</v>
+      </c>
+      <c r="D9" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>04/17/2025</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>647.2130799999995</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.07725431012611803</v>
+      </c>
+      <c r="D10" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
         <v>45765</v>
       </c>
-      <c r="B11">
-        <v>638.10400000000004</v>
-      </c>
-      <c r="C11">
-        <v>7.6840000000000006E-2</v>
-      </c>
-      <c r="D11">
+      <c r="B11" t="n">
+        <v>638.104</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.07684000000000001</v>
+      </c>
+      <c r="D11" t="n">
         <v>49.03</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>04/19/2025</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>642.3659099999995</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.07783725633883659</v>
+      </c>
+      <c r="D12" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-04-22
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,6 +617,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>04/22/2025</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>540.8340000000007</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.09244980899869448</v>
+      </c>
+      <c r="D13" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-04-24
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,6 +633,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>04/24/2025</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>509.2249999999985</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.09818842358485963</v>
+      </c>
+      <c r="D14" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-04-29
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,6 +679,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>04/29/2025</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>535.3930000000037</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.09338934203472898</v>
+      </c>
+      <c r="D17" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-01
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -695,6 +695,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>05/01/2025</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>524.0279999999984</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.09541474883021546</v>
+      </c>
+      <c r="D18" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-03
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,6 +711,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>05/03/2025</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>512.6880000000019</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.09752520051181189</v>
+      </c>
+      <c r="D19" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-06
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -727,6 +727,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>05/06/2025</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>550.3459999999977</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.09085193678158869</v>
+      </c>
+      <c r="D20" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-08
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,6 +743,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>05/08/2025</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>510.1650000000009</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.09800750737506476</v>
+      </c>
+      <c r="D21" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-10
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -759,6 +759,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>05/10/2025</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>469.2189999999973</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.1065600497848559</v>
+      </c>
+      <c r="D22" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-13
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,6 +775,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>05/13/2025</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>399.2560000000012</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.1252329332558555</v>
+      </c>
+      <c r="D23" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-15
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,6 +791,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>05/15/2025</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>414.3919999999998</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.120658699974903</v>
+      </c>
+      <c r="D24" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-17
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -807,6 +807,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>05/17/2025</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>448.8969999999972</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.1113841259799025</v>
+      </c>
+      <c r="D25" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-20
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,6 +823,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>05/20/2025</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>459.3410000000003</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.1088515939138896</v>
+      </c>
+      <c r="D26" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-22
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,6 +839,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>05/22/2025</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>422.9830000000002</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.1182080603712205</v>
+      </c>
+      <c r="D27" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-24
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +855,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>05/24/2025</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>454.8550000000032</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.1099251409789925</v>
+      </c>
+      <c r="D28" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-05-29
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,6 +871,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>05/29/2025</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>508.9639999999999</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.09823877523754138</v>
+      </c>
+      <c r="D29" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-06-20
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -947,6 +947,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>06/20/2025</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>713.8940000000002</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.07003840906353041</v>
+      </c>
+      <c r="D34" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-06-22
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -963,6 +963,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>06/22/2025</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>155.4730000000054</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.06431984974882875</v>
+      </c>
+      <c r="D35" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-06-27
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -979,6 +979,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>06/27/2025</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>674.4099999999962</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.07413887694429247</v>
+      </c>
+      <c r="D36" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-06-29
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -995,6 +995,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>06/29/2025</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>127.8790000000008</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.07819892241884857</v>
+      </c>
+      <c r="D37" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-07-04
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1011,6 +1011,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>07/04/2025</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>629.2050000000017</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.0794653570775818</v>
+      </c>
+      <c r="D38" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-07-06
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1027,6 +1027,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>07/06/2025</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>131.3220000000001</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.07614870318758465</v>
+      </c>
+      <c r="D39" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-07-18
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1073,6 +1073,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>07/18/2025</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>520.4100000000035</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.09607809227339917</v>
+      </c>
+      <c r="D42" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-07-20
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1089,6 +1089,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>07/20/2025</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>100.8229999999967</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.09918371800085625</v>
+      </c>
+      <c r="D43" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-07-25
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1105,6 +1105,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>07/25/2025</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>499.4599999999991</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.1001081167661076</v>
+      </c>
+      <c r="D44" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-07-27
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1121,6 +1121,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>07/27/2025</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>93.56999999999971</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.1068718606390941</v>
+      </c>
+      <c r="D45" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-01
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1137,6 +1137,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>08/01/2025</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>556.875</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.08978675645342311</v>
+      </c>
+      <c r="D46" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-03
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1153,6 +1153,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>08/03/2025</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>115.5390000000043</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.08655086161382414</v>
+      </c>
+      <c r="D47" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-08
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1169,6 +1169,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>08/08/2025</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>552.2389999999941</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.09054050872901141</v>
+      </c>
+      <c r="D48" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-10
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1185,6 +1185,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>08/10/2025</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>107.096000000005</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.0933741689698918</v>
+      </c>
+      <c r="D49" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-15
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1201,6 +1201,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>08/15/2025</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>550.1630000000005</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.09088215674263801</v>
+      </c>
+      <c r="D50" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-17
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1217,6 +1217,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>08/17/2025</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>106.9919999999984</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.09346493195753096</v>
+      </c>
+      <c r="D51" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-22
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1233,6 +1233,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>08/22/2025</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>578.1140000000014</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.08648813209851323</v>
+      </c>
+      <c r="D52" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-24
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1249,6 +1249,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>08/24/2025</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>112.0649999999951</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.08923392673895009</v>
+      </c>
+      <c r="D53" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-29
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -1,76 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding_stuff\crypto_buys\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB015EC-BE1D-4BDB-A95D-6AF8925019F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Coins</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -85,44 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -410,70 +420,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Coins</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08/29/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>557.5866699999997</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.08967215805212853</v>
+      </c>
+      <c r="D2" t="n">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-08-31
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08/31/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>116.8280000000004</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.08559591878659194</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-09-05
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +487,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>603.0450000000001</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.08291255213126714</v>
+      </c>
+      <c r="D4" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-09-12
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,6 +503,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>09/12/2025</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>862.7109999999993</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.05795683606677095</v>
+      </c>
+      <c r="D5" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-09-26
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -1,72 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding_stuff\crypto_buys\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22CFD72-AFD7-41F8-B3E9-439301B4F578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Coins</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>08/29/2025</t>
-  </si>
-  <si>
-    <t>08/31/2025</t>
-  </si>
-  <si>
-    <t>09/05/2025</t>
-  </si>
-  <si>
-    <t>09/12/2025</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -81,44 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -406,99 +424,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>557.58666999999969</v>
-      </c>
-      <c r="C2">
-        <v>8.9672158052128526E-2</v>
-      </c>
-      <c r="D2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Coins</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08/29/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>557.5866699999997</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.08967215805212853</v>
+      </c>
+      <c r="D2" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>08/31/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>116.8280000000004</v>
       </c>
-      <c r="C3">
-        <v>8.5595918786591937E-2</v>
-      </c>
-      <c r="D3">
+      <c r="C3" t="n">
+        <v>0.08559591878659194</v>
+      </c>
+      <c r="D3" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>603.04500000000007</v>
-      </c>
-      <c r="C4">
-        <v>8.2912552131267137E-2</v>
-      </c>
-      <c r="D4">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>603.0450000000001</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.08291255213126714</v>
+      </c>
+      <c r="D4" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>09/12/2025</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>286.62</v>
       </c>
-      <c r="C5">
-        <v>8.7220000000000006E-2</v>
-      </c>
-      <c r="D5">
+      <c r="C5" t="n">
+        <v>0.08722000000000001</v>
+      </c>
+      <c r="D5" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>45919</v>
       </c>
-      <c r="B6">
-        <v>282.69200000000001</v>
-      </c>
-      <c r="C6">
-        <v>8.8440000000000005E-2</v>
-      </c>
-      <c r="D6">
+      <c r="B6" t="n">
+        <v>282.692</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.08844</v>
+      </c>
+      <c r="D6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>09/26/2025</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>307.6989999999996</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1624964657018712</v>
+      </c>
+      <c r="D7" t="n">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-10-03
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,6 +553,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>10/03/2025</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>304.5709999999999</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1641653341913709</v>
+      </c>
+      <c r="D8" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-10-10
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -569,6 +569,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>10/10/2025</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>335.1719999999996</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1491771389018178</v>
+      </c>
+      <c r="D9" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-10-17
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,6 +585,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>10/17/2025</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>463.9639999999999</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.1077669819210111</v>
+      </c>
+      <c r="D10" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-10-24
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -601,6 +601,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10/24/2025</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>482.9750000000004</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.1035250271753196</v>
+      </c>
+      <c r="D11" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-11-07
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -633,6 +633,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>11/07/2025</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>494.851999999999</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.05001495396603439</v>
+      </c>
+      <c r="D13" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-11-14
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,6 +649,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>11/14/2025</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>507.4490000000005</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.04877337427012365</v>
+      </c>
+      <c r="D14" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-11-21
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,6 +665,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>11/21/2025</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>594.4650000000001</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.04163407433574726</v>
+      </c>
+      <c r="D15" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-11-28
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -681,6 +681,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>11/28/2025</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>418.3989999999994</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.05915406107567187</v>
+      </c>
+      <c r="D16" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-12-19
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -727,6 +727,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>12/19/2025</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>600.8780000000006</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.04118972570139025</v>
+      </c>
+      <c r="D19" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2025-12-26
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,6 +743,22 @@
         <v>25</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>12/26/2025</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1120.191999999999</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.04418885333942756</v>
+      </c>
+      <c r="D20" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2026-01-02
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -759,6 +759,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>01/02/2026</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1101.564</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.04493610902317068</v>
+      </c>
+      <c r="D21" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2026-01-09
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,6 +775,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>01/09/2026</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1039.873</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.04760196677863548</v>
+      </c>
+      <c r="D22" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2026-01-16
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,6 +791,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>01/16/2026</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1076.170999999998</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.04599640763410282</v>
+      </c>
+      <c r="D23" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2026-01-23
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -807,6 +807,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>01/23/2026</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1133.198</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.04368168669552892</v>
+      </c>
+      <c r="D24" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2026-01-30
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,6 +823,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>01/30/2026</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1275.224000000002</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.03881670984862261</v>
+      </c>
+      <c r="D25" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2026-02-06
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,6 +839,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>02/06/2026</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1767.745999999999</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0280017604339085</v>
+      </c>
+      <c r="D26" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2026-02-13
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +855,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>02/13/2026</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1553.712000000001</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.03185918625845714</v>
+      </c>
+      <c r="D27" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2026-02-20
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,6 +871,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>02/20/2026</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1623.165999999997</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0304959566674019</v>
+      </c>
+      <c r="D28" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update kaspa_buys.xlsx after running on 2026-02-27
</commit_message>
<xml_diff>
--- a/data/kaspa_buys.xlsx
+++ b/data/kaspa_buys.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -887,6 +887,22 @@
         <v>50</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>02/27/2026</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1557.662000000004</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.03177839608336075</v>
+      </c>
+      <c r="D29" t="n">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>